<commit_message>
Update theoretical analysis of methods.xlsx
</commit_message>
<xml_diff>
--- a/DataProject/theoretical analysis of methods.xlsx
+++ b/DataProject/theoretical analysis of methods.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Kaya\Desktop\dataproject\vacation_management\DataProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8062DF2F-B161-489E-A4E5-DBB9B4C57C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="5565" yWindow="2220" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Class_ Admin - Class_" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 2 - Class_ Customer - Cla" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet 3 - Class_ TourManager - " sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet 4 - Class_ HotelManager -" sheetId="4" r:id="rId7"/>
+    <sheet name="Sheet 1 - Class_ Admin - Class_" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 2 - Class_ Customer - Cla" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet 3 - Class_ TourManager - " sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet 4 - Class_ HotelManager -" sheetId="4" r:id="rId4"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Class: Admin</t>
   </si>
@@ -80,9 +89,6 @@
   </si>
   <si>
     <t>cancelTicket</t>
-  </si>
-  <si>
-    <t>checkDates</t>
   </si>
   <si>
     <t>leaveCommentToHotel</t>
@@ -133,29 +139,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
@@ -376,66 +374,69 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -446,27 +447,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ff00a2ff"/>
-      <rgbColor rgb="ffc8c8c8"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff89847f"/>
-      <rgbColor rgb="fff7f7f6"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FF00A2FF"/>
+      <rgbColor rgb="FFC8C8C8"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF89847F"/>
+      <rgbColor rgb="FFF7F7F6"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -665,7 +724,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -684,7 +743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -714,7 +773,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -740,7 +799,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -766,7 +825,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -792,7 +851,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -818,7 +877,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -844,7 +903,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -870,7 +929,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -896,7 +955,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -922,7 +981,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -935,9 +994,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -954,7 +1019,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -973,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -999,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1025,7 +1090,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1051,7 +1116,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1077,7 +1142,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1103,7 +1168,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1129,7 +1194,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1155,7 +1220,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1181,7 +1246,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1207,7 +1272,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1220,9 +1285,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1236,7 +1307,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1255,7 +1326,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1285,7 +1356,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1311,7 +1382,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1337,7 +1408,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1363,7 +1434,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1389,7 +1460,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1415,7 +1486,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1441,7 +1512,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1467,7 +1538,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1493,7 +1564,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1506,166 +1577,176 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="24.6562" style="1" customWidth="1"/>
-    <col min="2" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
+    <col min="2" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="11">
+      <c r="B3" s="5"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="11">
+      <c r="B4" s="7"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="11">
+      <c r="B5" s="8"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="11">
+      <c r="B6" s="7"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" t="s" s="11">
+      <c r="B7" s="8"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" t="s" s="11">
+      <c r="B8" s="7"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="11">
+      <c r="B9" s="8"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="11">
+      <c r="B10" s="7"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="11">
+      <c r="B11" s="8"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" ht="20.2" customHeight="1">
-      <c r="A13" t="s" s="11">
+      <c r="B12" s="7"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" ht="20.2" customHeight="1">
-      <c r="A14" t="s" s="11">
+      <c r="B13" s="8"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1673,203 +1754,197 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.1797" style="16" customWidth="1"/>
-    <col min="2" max="4" width="16.3516" style="16" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="16" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="9" customWidth="1"/>
+    <col min="2" max="5" width="16.28515625" style="9" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="5">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="8">
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="11">
+      <c r="B3" s="5"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="11">
+      <c r="B4" s="7"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="11">
+      <c r="B5" s="8"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="11">
+      <c r="B6" s="7"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" t="s" s="11">
+      <c r="B7" s="8"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="8"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" t="s" s="11">
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="11">
+      <c r="B9" s="7"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="11">
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="11">
+      <c r="B11" s="7"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" ht="20.2" customHeight="1">
-      <c r="A13" t="s" s="11">
+    <row r="13" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" ht="20.2" customHeight="1">
-      <c r="A14" t="s" s="11">
+      <c r="B13" s="7"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="12"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
     </row>
-    <row r="15" ht="20.2" customHeight="1">
-      <c r="A15" t="s" s="11">
+    <row r="15" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" ht="20.2" customHeight="1">
-      <c r="A16" t="s" s="11">
+      <c r="B15" s="7"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
     </row>
-    <row r="17" ht="20.2" customHeight="1">
-      <c r="A17" t="s" s="11">
+    <row r="17" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" ht="20.2" customHeight="1">
-      <c r="A18" t="s" s="11">
+      <c r="B17" s="7"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="12"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
     </row>
-    <row r="19" ht="20.2" customHeight="1">
-      <c r="A19" t="s" s="11">
-        <v>33</v>
-      </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-    </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="18">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C15:D15"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1877,86 +1952,89 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.1797" style="17" customWidth="1"/>
-    <col min="2" max="4" width="16.3516" style="17" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="17" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="10" customWidth="1"/>
+    <col min="2" max="5" width="16.28515625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="11">
-        <v>14</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="11">
-        <v>9</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="11">
-        <v>35</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -1964,86 +2042,89 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.1797" style="18" customWidth="1"/>
-    <col min="2" max="4" width="16.3516" style="18" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="18" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" style="11" customWidth="1"/>
+    <col min="2" max="5" width="16.28515625" style="11" customWidth="1"/>
+    <col min="6" max="16384" width="16.28515625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.15" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:4" ht="23.1" customHeight="1">
+      <c r="A1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" ht="20.45" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
+      <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="6">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="8">
-        <v>4</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="11">
-        <v>8</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="11">
-        <v>37</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>